<commit_message>
creazione file train_timetable e inserimento dei dati nel database Public Transportation. Modifiche alla classe CreateJSONfile
</commit_message>
<xml_diff>
--- a/Java/BGTransport/src/main/resources/excel/list/train_station_list.xlsx
+++ b/Java/BGTransport/src/main/resources/excel/list/train_station_list.xlsx
@@ -1,42 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/86d5980519d90a03/Desktop/BGTransports/Java/BGTransport/src/main/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utente\Desktop\BGTransports\Java\BGTransport\src\main\resources\excel\list\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{AB8B8952-1495-40AA-9908-2C0BDC3EAF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{96E0759E-F42F-4B94-AE34-8714FB035B6C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A0CEEB6-055C-4D94-904F-043D6EBCDBAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8D5B4CB3-3E46-453F-BD73-C4424EF1706F}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="140">
   <si>
     <t>Albano S.Alessandro</t>
   </si>
@@ -80,9 +69,6 @@
     <t>Calusco</t>
   </si>
   <si>
-    <t>V. Trieste, 22</t>
-  </si>
-  <si>
     <t>Calusco D'adda</t>
   </si>
   <si>
@@ -95,9 +81,6 @@
     <t>Chiuduno</t>
   </si>
   <si>
-    <t>V. Monsignor Valoti</t>
-  </si>
-  <si>
     <t>Cisano-Caprino Bergamasco</t>
   </si>
   <si>
@@ -110,9 +93,6 @@
     <t>Cividate-Calcio</t>
   </si>
   <si>
-    <t>V. Stazione</t>
-  </si>
-  <si>
     <t>Cividate Al Piano</t>
   </si>
   <si>
@@ -134,18 +114,12 @@
     <t>Montello-Gorlago</t>
   </si>
   <si>
-    <t>V. Stazione, 6</t>
-  </si>
-  <si>
     <t>Montello</t>
   </si>
   <si>
     <t>Morengo-Bariano</t>
   </si>
   <si>
-    <t>V. Locatelli</t>
-  </si>
-  <si>
     <t>Bariano</t>
   </si>
   <si>
@@ -173,9 +147,6 @@
     <t>Seriate</t>
   </si>
   <si>
-    <t>V. Stazione, 2</t>
-  </si>
-  <si>
     <t>Stezzano</t>
   </si>
   <si>
@@ -185,9 +156,6 @@
     <t>Terno</t>
   </si>
   <si>
-    <t>V. Marconi, 14</t>
-  </si>
-  <si>
     <t>Terno D'isola</t>
   </si>
   <si>
@@ -206,18 +174,12 @@
     <t>Verdello-Dalmine</t>
   </si>
   <si>
-    <t>V. Marconi, 54</t>
-  </si>
-  <si>
     <t>Verdellino</t>
   </si>
   <si>
     <t>Vidalengo</t>
   </si>
   <si>
-    <t>V. Donizetti</t>
-  </si>
-  <si>
     <t>name</t>
   </si>
   <si>
@@ -228,13 +190,268 @@
   </si>
   <si>
     <t>province</t>
+  </si>
+  <si>
+    <t>Palazzolo sull'Oglio</t>
+  </si>
+  <si>
+    <t>Cologne</t>
+  </si>
+  <si>
+    <t>Coccaglio</t>
+  </si>
+  <si>
+    <t>Rovato</t>
+  </si>
+  <si>
+    <t>Ospitaletto</t>
+  </si>
+  <si>
+    <t>Brescia</t>
+  </si>
+  <si>
+    <t>Via Guglielmo Marconi, 100</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Via Donizetti</t>
+  </si>
+  <si>
+    <t>Via Trieste, 22</t>
+  </si>
+  <si>
+    <t>Via Monsignor Valoti</t>
+  </si>
+  <si>
+    <t>Via Stazione</t>
+  </si>
+  <si>
+    <t>Via Stazione, 6</t>
+  </si>
+  <si>
+    <t>Via Locatelli</t>
+  </si>
+  <si>
+    <t>Via Stazione, 2</t>
+  </si>
+  <si>
+    <t>Via Marconi, 14</t>
+  </si>
+  <si>
+    <t>Via Marconi, 54</t>
+  </si>
+  <si>
+    <t>Via Roma, 141</t>
+  </si>
+  <si>
+    <t>Viale Giacomo Matteotti, 14</t>
+  </si>
+  <si>
+    <t>Viale Lombardia, 10</t>
+  </si>
+  <si>
+    <t>Via Martiri della Libertà (SP19), 183</t>
+  </si>
+  <si>
+    <t>Viale della Stazione, 54</t>
+  </si>
+  <si>
+    <t>Arcore</t>
+  </si>
+  <si>
+    <t>Monza</t>
+  </si>
+  <si>
+    <t>Sesto San Giovanni</t>
+  </si>
+  <si>
+    <t>Milano Greco Pirelli</t>
+  </si>
+  <si>
+    <t>Milano Porta Garibaldi</t>
+  </si>
+  <si>
+    <t>Viale Libertà, 1</t>
+  </si>
+  <si>
+    <t>Paderno d'Adda</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Via Roma, 2</t>
+  </si>
+  <si>
+    <t>Carnate</t>
+  </si>
+  <si>
+    <t>Milano</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>Piazzale Martire della Libertà</t>
+  </si>
+  <si>
+    <t>Via Enrico Arosio, 14</t>
+  </si>
+  <si>
+    <t>Piazza I Maggio, 1</t>
+  </si>
+  <si>
+    <t>MI</t>
+  </si>
+  <si>
+    <t>Piazzale Egeo</t>
+  </si>
+  <si>
+    <t>Piazza Sigmund Freud, 1</t>
+  </si>
+  <si>
+    <t>Ospitaletto-Travagliato</t>
+  </si>
+  <si>
+    <t>Paderno-Robbiate</t>
+  </si>
+  <si>
+    <t>Carnate-Usmate</t>
+  </si>
+  <si>
+    <t>Calolziocorte-Olginate</t>
+  </si>
+  <si>
+    <t>Via Attilio Galli, 15</t>
+  </si>
+  <si>
+    <t>Calolziocorte</t>
+  </si>
+  <si>
+    <t>Vercurago San Girolamo</t>
+  </si>
+  <si>
+    <t>Lecco-Maggianico</t>
+  </si>
+  <si>
+    <t>Lecco</t>
+  </si>
+  <si>
+    <t>Via IV Novembre, 25</t>
+  </si>
+  <si>
+    <t>Vercurago</t>
+  </si>
+  <si>
+    <t>Via Antonio Carlo Gomez, 15</t>
+  </si>
+  <si>
+    <t>Piazza Stazione</t>
+  </si>
+  <si>
+    <t>Pioltello-Limito</t>
+  </si>
+  <si>
+    <t>Milano Lambrate</t>
+  </si>
+  <si>
+    <t>Milano Villapizzone</t>
+  </si>
+  <si>
+    <t>Milano Centrale</t>
+  </si>
+  <si>
+    <t>Via alla Stazione, 1</t>
+  </si>
+  <si>
+    <t>Pioltello</t>
+  </si>
+  <si>
+    <t>Piazza Enrico Bottini, 10</t>
+  </si>
+  <si>
+    <t>Via Arnaldo Fusinato, 26</t>
+  </si>
+  <si>
+    <t>Piazza Duca d'Aosta</t>
+  </si>
+  <si>
+    <t>Milano Certosa</t>
+  </si>
+  <si>
+    <t>Milano Lancetti</t>
+  </si>
+  <si>
+    <t>Milano Porta Garibaldi Passante</t>
+  </si>
+  <si>
+    <t>Milano Repubblica</t>
+  </si>
+  <si>
+    <t>Milano Porta Venezia</t>
+  </si>
+  <si>
+    <t>Milano Dateo</t>
+  </si>
+  <si>
+    <t>Milano Porta Vittoria</t>
+  </si>
+  <si>
+    <t>Milano Forlanini</t>
+  </si>
+  <si>
+    <t>Segrate</t>
+  </si>
+  <si>
+    <t>Vignate</t>
+  </si>
+  <si>
+    <t>Melzo</t>
+  </si>
+  <si>
+    <t>Pozzuolo Martesana</t>
+  </si>
+  <si>
+    <t>Tracella</t>
+  </si>
+  <si>
+    <t>Cassano d'Adda</t>
+  </si>
+  <si>
+    <t>Piazza Gobetti</t>
+  </si>
+  <si>
+    <t>Via Marco Bruto</t>
+  </si>
+  <si>
+    <t>Via Cervignano</t>
+  </si>
+  <si>
+    <t>Viale Piceno</t>
+  </si>
+  <si>
+    <t>Corso Buenos Aires</t>
+  </si>
+  <si>
+    <t>Piazza della Repubblica</t>
+  </si>
+  <si>
+    <t>Piazza Sigmund Freud</t>
+  </si>
+  <si>
+    <t>Via Lancetti</t>
+  </si>
+  <si>
+    <t>Via Triboniano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -292,26 +509,6 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -409,6 +606,26 @@
       <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -423,13 +640,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E703F1C-E07E-487D-A6B0-B297D44D29C1}" name="Tabella1" displayName="Tabella1" ref="A1:D25" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:D25" xr:uid="{8E703F1C-E07E-487D-A6B0-B297D44D29C1}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8E703F1C-E07E-487D-A6B0-B297D44D29C1}" name="Tabella1" displayName="Tabella1" ref="A1:D60" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D60" xr:uid="{8E703F1C-E07E-487D-A6B0-B297D44D29C1}"/>
+  <sortState ref="A2:D60">
+    <sortCondition ref="A1:A60"/>
+  </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{E50CCA0F-B3E2-4BAF-8B18-CCF4A989B7B2}" name="name" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{66568630-A378-4056-9BA6-B3E7E4F9F3CE}" name="address" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{649E33F3-C286-483C-B992-05A27C134AEA}" name="town" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{BDE1BC28-8EBE-48C4-8BEA-BC2DCEA6AB9E}" name="province" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E50CCA0F-B3E2-4BAF-8B18-CCF4A989B7B2}" name="name" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{66568630-A378-4056-9BA6-B3E7E4F9F3CE}" name="address" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{649E33F3-C286-483C-B992-05A27C134AEA}" name="town" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{BDE1BC28-8EBE-48C4-8BEA-BC2DCEA6AB9E}" name="province" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -752,35 +972,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30E33295-D896-4A72-8370-492C4232BF8E}">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="26" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.8984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.8984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="14.4">
       <c r="A1" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="14.4">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -794,7 +1014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="14.4">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -808,7 +1028,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="14.4">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -822,26 +1042,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="14.4">
       <c r="A5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="14.4">
+      <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>9</v>
@@ -850,270 +1070,760 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="14.4">
       <c r="A7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.4">
+      <c r="A8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="14.4">
+      <c r="A9" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="14.4">
+      <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B10" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="D10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="14.4">
+      <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="14.4">
+      <c r="A12" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="14.4">
+      <c r="A13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.4">
+      <c r="A14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="14.4">
+      <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.4">
+      <c r="A16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="B16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="14.4">
+      <c r="A17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="14.4">
+      <c r="A18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="14.4">
+      <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C19" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="D19" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.4">
+      <c r="A20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="14.4">
+      <c r="A21" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="14.4">
+      <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B22" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="14.4">
+      <c r="A23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="14.4">
+      <c r="A24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="14.4">
+      <c r="A25" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="14.4">
+      <c r="A26" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="14.4">
+      <c r="A27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="14.4">
+      <c r="A28" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="14.4">
+      <c r="A29" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="14.4">
+      <c r="A30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="14.4">
+      <c r="A31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14.4">
+      <c r="A32" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="14.4">
+      <c r="A33" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="14.4">
+      <c r="A34" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="14.4">
+      <c r="A35" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="14.4">
+      <c r="A36" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="14.4">
+      <c r="A37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="D37" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="14.4">
+      <c r="A38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="14.4">
+      <c r="A39" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B39" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D39" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="14.4">
+      <c r="A40" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="14.4">
+      <c r="A41" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="14.4">
+      <c r="A42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="14.4">
+      <c r="A43" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="14.4">
+      <c r="A44" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="B44" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="C44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="D44" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="14.4">
+      <c r="A45" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="B45" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="14.4">
+      <c r="A46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="14.4">
+      <c r="A47" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B47" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D47" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="14.4">
+      <c r="A48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="14.4">
+      <c r="A49" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="14.4">
+      <c r="A50" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B50" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="14.4">
+      <c r="A51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="14.4">
+      <c r="A52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B52" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="D52" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="14.4">
+      <c r="A53" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="B53" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C53" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="D53" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="14.4">
+      <c r="A54" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="14.4">
+      <c r="A55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B55" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="D55" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="14.4">
+      <c r="A56" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B56" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="C56" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="14.4">
+      <c r="A57" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="14.4">
+      <c r="A58" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B58" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="D58" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="14.4">
+      <c r="A59" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>3</v>
+      <c r="B59" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="14.4">
+      <c r="A60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>